<commit_message>
starter code for breakpoints analysis
</commit_message>
<xml_diff>
--- a/stats_region.xlsx
+++ b/stats_region.xlsx
@@ -451,25 +451,25 @@
         <v>43871</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>45017</v>
+        <v>44907</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0126256363620472</v>
+        <v>0.0135406646415844</v>
       </c>
       <c r="G2" t="n">
-        <v>0.699136370231584</v>
+        <v>1.00619485639197</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.00198514565936229</v>
+        <v>0.00196336990767471</v>
       </c>
       <c r="J2" t="n">
-        <v>0.00820514375731883</v>
+        <v>0.00861649090764852</v>
       </c>
       <c r="K2" t="n">
-        <v>0.000426522820766044</v>
+        <v>0.000414262513320785</v>
       </c>
     </row>
     <row r="3">
@@ -486,25 +486,25 @@
         <v>43871</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>45017</v>
+        <v>44907</v>
       </c>
       <c r="F3" t="n">
-        <v>0.101454371391784</v>
+        <v>0.103935692392368</v>
       </c>
       <c r="G3" t="n">
-        <v>1.13330533789194</v>
+        <v>1.39045246368396</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0456307540447083</v>
+        <v>0.0457945946206097</v>
       </c>
       <c r="J3" t="n">
-        <v>0.136340689407087</v>
+        <v>0.137297394402522</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0140840514243875</v>
+        <v>0.0137871562209999</v>
       </c>
     </row>
     <row r="4">
@@ -521,25 +521,25 @@
         <v>43871</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>45017</v>
+        <v>44907</v>
       </c>
       <c r="F4" t="n">
-        <v>0.10767691033591</v>
+        <v>0.112483257021618</v>
       </c>
       <c r="G4" t="n">
-        <v>1.97964956682087</v>
+        <v>2.40966284884659</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0112411527964102</v>
+        <v>-0.0119310649580203</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0396008002137674</v>
+        <v>0.0392412304075698</v>
       </c>
       <c r="J4" t="n">
-        <v>0.143768739092944</v>
+        <v>0.144118176905062</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00611236459907884</v>
+        <v>0.00598365806940942</v>
       </c>
     </row>
     <row r="5">
@@ -556,25 +556,25 @@
         <v>43871</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>45017</v>
+        <v>44907</v>
       </c>
       <c r="F5" t="n">
-        <v>0.279812057291336</v>
+        <v>0.290083895429395</v>
       </c>
       <c r="G5" t="n">
-        <v>11.2169312169312</v>
+        <v>14.2222222222222</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.188894558496374</v>
+        <v>0.186934849799873</v>
       </c>
       <c r="J5" t="n">
-        <v>0.390726341858326</v>
+        <v>0.392035473943881</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0737611479916851</v>
+        <v>0.0722292075782106</v>
       </c>
     </row>
     <row r="6">
@@ -588,28 +588,28 @@
         <v>5019</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>43871</v>
+        <v>43878</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>45017</v>
+        <v>44907</v>
       </c>
       <c r="F6" t="n">
-        <v>0.131162999966067</v>
+        <v>0.135210958198813</v>
       </c>
       <c r="G6" t="n">
-        <v>1.55888967620691</v>
+        <v>1.74235782893734</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0293556436224864</v>
+        <v>0.0290100042592723</v>
       </c>
       <c r="J6" t="n">
-        <v>0.166290129724143</v>
+        <v>0.166449080132706</v>
       </c>
       <c r="K6" t="n">
-        <v>0.00143286481644322</v>
+        <v>0.0013281937486539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>